<commit_message>
Updated Excel for Varddokument.
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vårddokument.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vårddokument.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="282">
   <si>
     <t>Meddelandestruktur</t>
   </si>
@@ -555,12 +555,6 @@
 Använd identitet MM1, MM2, MM3 och så vidare.</t>
   </si>
   <si>
-    <t>Själva anteckningen. Anteckningen kan innehålla platshållare för multimediaobjekt som medföljer dokumentet, om multimediaobjektet ska bäddas in i anteckningstexten. Själva multimediaobjektet definieras i &lt;multimediaEntry&gt;. Formatet på platshållaren är &lt;renderMultiMedia referencedObject="id"/&gt;, där id är identiteten på multimediaobjektet (exempelvis "MM1"), som definieras i &lt;multimediaEntry&gt;.</t>
-  </si>
-  <si>
-    <t>Multimediaobjekt som medföljer dokumentet. Varje sådant multimediaobjekt kan motsvaras av en platshållare i clinicalDocumentNoteText.</t>
-  </si>
-  <si>
     <t>Dokumentets identitet som är unik inom källsystemet</t>
   </si>
   <si>
@@ -568,9 +562,6 @@
   </si>
   <si>
     <t>Information om den hälso- och sjukvårdsperson som skapat informationen i dokumentet, nedan kallas författare.</t>
-  </si>
-  <si>
-    <t>Kod för författarens befattning. Tillåtna värden från kodverk Befattning (OID 1.2.752.129.2.2.1.4) , se http://www.inera.se/Documents/Infrastrukturtjanster/Katalogtjanst_HSA/Innehll/hsa_innehall_befattning.pdf</t>
   </si>
   <si>
     <t>Information om vem som signerat informationen i dokumentet.</t>
@@ -711,9 +702,6 @@
     <t>vård-och omsorgsdokument.registreringstidpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">enhet.enhets-id </t>
-  </si>
-  <si>
     <t>enhet.postadress</t>
   </si>
   <si>
@@ -739,9 +727,6 @@
 clinicalDocument.author.assignedAuthor.representedOrganization.id.root = 1.2.752.129.2.1.4.1</t>
   </si>
   <si>
-    <t>clinicalDocument.author.assignedAuthor.representedOrganization.addr = PatientSummaryHeader.author.careUnitHSAddress</t>
-  </si>
-  <si>
     <t>clinicalDocument.author.assignedAuthor.representedOrganization.asOrganizationPartOf.wholeOrganization.id.extention = PatientSummaryHeader.author.careGiverHSAid
 clinicalDocument.author.assignedAuthor.representedOrganization.asOrganizationPartOf.wholeOrganization.id.root = 1.2.752.129.2.1.4.1</t>
   </si>
@@ -753,11 +738,6 @@
 clinicalDocument.legalAuthenticator.assignedEntity.id.root = 1.2.752.129.2.1.4.1</t>
   </si>
   <si>
-    <t>clinicalDocument.legalAuthenticator.assignedEntity.representedOrganization.id.extention = PatientSummaryHeader.author.careUnitHSAid
-clinicalDocument.legalAuthenticator.assignedEntity.representedOrganization.id.root = 1.2.752.129.2.1.4.1
-Not: clinicalDocumet.legalAuthenticator.assignedEntity ska ha samma värde på organisation som clinicalDocument.author.assignedAuthor.representedOrganization</t>
-  </si>
-  <si>
     <t>Om approvedForPatient är true skapas clinicalDocument.authorization samt sätts clinicalDocument.authorization.consent.code till "P0.00790" samt .codeSystem till "2.16.840.1.113883.6.96"
 Om approvedForPatient är false skapas ej clinicalDocument.authorization</t>
   </si>
@@ -836,19 +816,77 @@
     <t>authorOrgUnitname</t>
   </si>
   <si>
-    <t>Namnet på den organisation som författaren är updragsgivare</t>
-  </si>
-  <si>
     <t>Postadress för den organisation som författaren är uppdragsgivare på.</t>
   </si>
   <si>
-    <t>Tidsangivelse för den händelse dokumentet gäller</t>
-  </si>
-  <si>
     <t>vård-och omsorgsdokument.händelsetidpunkt</t>
   </si>
   <si>
     <t>authorOrgUnitAddress</t>
+  </si>
+  <si>
+    <t>informationsmängd.systemid</t>
+  </si>
+  <si>
+    <t>vård-och omsorgsdokument.personal-id</t>
+  </si>
+  <si>
+    <t>vård-och omsorgsdokument.befattning</t>
+  </si>
+  <si>
+    <t>Den organisation som författaren är uppdragstagare på</t>
+  </si>
+  <si>
+    <t>Namnet på den organisation som författaren är updragsgivare på</t>
+  </si>
+  <si>
+    <t>enhet.enhets-id</t>
+  </si>
+  <si>
+    <t>enhet.enhetsnamn</t>
+  </si>
+  <si>
+    <t>ingen mappning</t>
+  </si>
+  <si>
+    <t>Vård- och omsorgsdokument.innehåll text</t>
+  </si>
+  <si>
+    <t>Vård- och omsorgsdokument.innehåll multimedia</t>
+  </si>
+  <si>
+    <t>Dokumentets innehåll i text</t>
+  </si>
+  <si>
+    <t>Länk till dokumentets innehåll i form av en multimediafil</t>
+  </si>
+  <si>
+    <t>Händelsetidpunkt. Tidsangivelse för den händelse dokumentet gäller.</t>
+  </si>
+  <si>
+    <t>Tidpunkt då dokumentet skapades. .Det är den senaste tidpunkten då informationen uppdaterats i systemet som ska finnas här i de fall informationen har ändrats efter det att den skapades.</t>
+  </si>
+  <si>
+    <t>authorOtherRole</t>
+  </si>
+  <si>
+    <t>authorOtherRoleCode</t>
+  </si>
+  <si>
+    <t>authorOtherRoleCodeOID</t>
+  </si>
+  <si>
+    <t>Kod för författarens befattning enligt annat kodverk</t>
+  </si>
+  <si>
+    <t>Information om  författarens befattning om annat kodverk än KV Befattning används</t>
+  </si>
+  <si>
+    <t>OID för det kodverk som används för författarens befattning</t>
+  </si>
+  <si>
+    <t>Kod för författarens befattning. Tillåtna värden från kodverk Befattning (OID 1.2.752.129.2.2.1.4) , se http://www.inera.se/Documents/Infrastrukturtjanster/Katalogtjanst_HSA/Innehll/hsa_innehall_befattning.pdf
+I de fall inte KV Befattning kan användas kan authorOtherRole användas för att ange befattning enligt annat kodverk</t>
   </si>
 </sst>
 </file>
@@ -904,7 +942,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -953,6 +991,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -975,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1190,6 +1234,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1513,8 +1560,8 @@
   <dimension ref="A1:AT170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB29" sqref="AB29"/>
+      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB127" sqref="AB127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1609,8 +1656,8 @@
       <c r="U2" s="24"/>
       <c r="V2" s="34"/>
       <c r="W2" s="77"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
       <c r="Z2" s="42"/>
       <c r="AA2" s="42"/>
       <c r="AB2" s="42"/>
@@ -1634,48 +1681,48 @@
       <c r="AT2" s="2"/>
     </row>
     <row r="3" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="86"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="87"/>
       <c r="V3" s="74"/>
       <c r="W3" s="77" t="s">
-        <v>196</v>
-      </c>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87" t="s">
+        <v>193</v>
+      </c>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="88"/>
+      <c r="Z3" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="87"/>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="87"/>
-      <c r="AI3" s="87"/>
-      <c r="AJ3" s="87"/>
+      <c r="AA3" s="88"/>
+      <c r="AB3" s="88"/>
+      <c r="AC3" s="88"/>
+      <c r="AD3" s="88"/>
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="88"/>
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="88"/>
       <c r="AK3" s="35"/>
       <c r="AL3" s="36"/>
     </row>
@@ -1748,10 +1795,10 @@
         <v>37</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="W5" s="77" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="X5" s="38"/>
       <c r="Y5" s="38"/>
@@ -1902,10 +1949,10 @@
       <c r="V9" s="48"/>
       <c r="W9" s="82"/>
       <c r="X9" s="47" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AD9" s="47" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
@@ -1939,7 +1986,7 @@
       <c r="W10" s="82"/>
       <c r="X10" s="54"/>
       <c r="Y10" s="75" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AD10" s="16" t="s">
         <v>140</v>
@@ -2092,13 +2139,13 @@
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="V14" s="50" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W14" s="81" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="X14" s="50"/>
       <c r="Y14" s="50"/>
@@ -2116,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AH14" s="46"/>
     </row>
@@ -2342,24 +2389,26 @@
       <c r="S20" s="48"/>
       <c r="T20" s="35"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="50"/>
+      <c r="V20" s="85" t="s">
+        <v>261</v>
+      </c>
       <c r="W20" s="82"/>
       <c r="X20" s="15"/>
       <c r="Y20" s="15"/>
       <c r="Z20" s="44" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="AA20" s="44"/>
       <c r="AB20" s="44"/>
       <c r="AC20" s="44"/>
       <c r="AD20" s="44" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AF20" s="44" t="s">
         <v>1</v>
       </c>
       <c r="AG20" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
@@ -2390,30 +2439,31 @@
         <v>108</v>
       </c>
       <c r="U21" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="V21" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="W21" s="81" t="s">
-        <v>216</v>
+        <v>220</v>
+      </c>
+      <c r="W21" s="53" t="s">
+        <v>213</v>
       </c>
       <c r="X21" s="35"/>
       <c r="Y21" s="35"/>
-      <c r="Z21" s="44" t="s">
+      <c r="Z21" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="AA21" s="44"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="44"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
       <c r="AE21" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="AF21" s="44" t="s">
+      <c r="AF21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AG21" s="63" t="s">
-        <v>180</v>
+      <c r="AG21" s="46" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2485,13 +2535,13 @@
         <v>108</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="V23" s="50" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="W23" s="81" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
@@ -2508,10 +2558,10 @@
         <v>151</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG23" s="46" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2747,27 +2797,27 @@
       <c r="U29" s="8"/>
       <c r="V29" s="50"/>
       <c r="W29" s="81" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="X29" s="35"/>
       <c r="Y29" s="35"/>
       <c r="Z29" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE29" s="46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AF29" s="3" t="s">
         <v>130</v>
       </c>
       <c r="AG29" s="46" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AH29" s="46"/>
     </row>
@@ -2799,10 +2849,10 @@
         <v>108</v>
       </c>
       <c r="U30" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="V30" s="50" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="W30" s="82"/>
       <c r="X30" s="35"/>
@@ -2905,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="AG32" s="46" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2980,10 +3030,10 @@
         <v>114</v>
       </c>
       <c r="V34" s="50" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="W34" s="81" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="X34" s="15"/>
       <c r="Y34" s="15"/>
@@ -3003,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="AG34" s="53" t="s">
-        <v>115</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3117,9 +3167,11 @@
       <c r="U37" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="V37" s="50"/>
+      <c r="V37" s="85" t="s">
+        <v>262</v>
+      </c>
       <c r="W37" s="81" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="X37" s="53"/>
       <c r="Y37" s="53"/>
@@ -3214,9 +3266,11 @@
       <c r="U39" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="V39" s="50"/>
+      <c r="V39" s="85" t="s">
+        <v>263</v>
+      </c>
       <c r="W39" s="81" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="X39" s="54"/>
       <c r="Y39" s="54"/>
@@ -3234,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="AG39" s="46" t="s">
-        <v>182</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3272,13 +3326,20 @@
       <c r="X40" s="54"/>
       <c r="Y40" s="54"/>
       <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
+      <c r="AA40" s="3" t="s">
+        <v>275</v>
+      </c>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
       <c r="AE40" s="3"/>
-      <c r="AF40" s="3"/>
-      <c r="AG40" s="46"/>
+      <c r="AF40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG40" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH40" s="3"/>
     </row>
     <row r="41" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
@@ -3316,12 +3377,21 @@
       <c r="Y41" s="15"/>
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
-      <c r="AB41" s="3"/>
+      <c r="AB41" s="3" t="s">
+        <v>276</v>
+      </c>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="46"/>
+      <c r="AE41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="AH41" s="3"/>
     </row>
     <row r="42" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
@@ -3359,12 +3429,21 @@
       <c r="Y42" s="15"/>
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="3"/>
-      <c r="AG42" s="46"/>
+      <c r="AE42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="AH42" s="3"/>
     </row>
     <row r="43" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
@@ -3403,7 +3482,8 @@
       <c r="AD43" s="3"/>
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
-      <c r="AG43" s="46"/>
+      <c r="AG43" s="3"/>
+      <c r="AH43" s="3"/>
     </row>
     <row r="44" spans="1:34" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
@@ -3433,13 +3513,13 @@
         <v>108</v>
       </c>
       <c r="U44" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="V44" s="50" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="W44" s="81" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="X44" s="15"/>
       <c r="Y44" s="15"/>
@@ -3456,9 +3536,10 @@
       <c r="AF44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AG44" s="46" t="s">
+      <c r="AG44" s="3" t="s">
         <v>172</v>
       </c>
+      <c r="AH44" s="3"/>
     </row>
     <row r="45" spans="1:34" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
@@ -3482,13 +3563,15 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
       <c r="U45" s="10"/>
-      <c r="V45" s="50"/>
+      <c r="V45" s="85" t="s">
+        <v>266</v>
+      </c>
       <c r="W45" s="81"/>
       <c r="X45" s="15"/>
       <c r="Y45" s="15"/>
       <c r="Z45" s="3"/>
       <c r="AA45" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
@@ -3501,7 +3584,9 @@
       <c r="AF45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG45" s="46"/>
+      <c r="AG45" s="46" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="46" spans="1:34" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
@@ -3525,13 +3610,15 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
       <c r="U46" s="10"/>
-      <c r="V46" s="50"/>
+      <c r="V46" s="85" t="s">
+        <v>267</v>
+      </c>
       <c r="W46" s="81"/>
       <c r="X46" s="15"/>
       <c r="Y46" s="15"/>
       <c r="Z46" s="3"/>
       <c r="AA46" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
@@ -3543,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="AG46" s="46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:34" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3568,13 +3655,15 @@
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
       <c r="U47" s="10"/>
-      <c r="V47" s="50"/>
+      <c r="V47" s="85" t="s">
+        <v>222</v>
+      </c>
       <c r="W47" s="81"/>
       <c r="X47" s="15"/>
       <c r="Y47" s="15"/>
       <c r="Z47" s="3"/>
       <c r="AA47" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
@@ -3586,7 +3675,7 @@
         <v>2</v>
       </c>
       <c r="AG47" s="46" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:34" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3656,15 +3745,17 @@
       <c r="U49" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="V49" s="50"/>
+      <c r="V49" s="50" t="s">
+        <v>224</v>
+      </c>
       <c r="W49" s="81" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="X49" s="15"/>
       <c r="Y49" s="15"/>
       <c r="Z49" s="3"/>
       <c r="AA49" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
@@ -3707,11 +3798,9 @@
         <v>108</v>
       </c>
       <c r="U50" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="V50" s="50" t="s">
-        <v>225</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="V50" s="50"/>
       <c r="W50" s="82"/>
       <c r="X50" s="54"/>
       <c r="Y50" s="54"/>
@@ -3863,14 +3952,10 @@
         <v>108</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="V54" s="50" t="s">
-        <v>226</v>
-      </c>
-      <c r="W54" s="81" t="s">
-        <v>234</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="V54" s="50"/>
+      <c r="W54" s="81"/>
       <c r="X54" s="54"/>
       <c r="Y54" s="54"/>
       <c r="Z54" s="55"/>
@@ -4028,13 +4113,13 @@
         <v>108</v>
       </c>
       <c r="U58" s="30" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="V58" s="50" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="W58" s="81" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="X58" s="55"/>
       <c r="Y58" s="55"/>
@@ -4260,7 +4345,7 @@
       <c r="AF63" s="3"/>
       <c r="AG63" s="46"/>
     </row>
-    <row r="64" spans="1:36" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -4288,10 +4373,7 @@
         <v>108</v>
       </c>
       <c r="U64" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="V64" s="50" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="W64" s="82"/>
       <c r="X64" s="54"/>
@@ -4398,7 +4480,7 @@
         <v>2</v>
       </c>
       <c r="AG66" s="46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4468,13 +4550,13 @@
         <v>108</v>
       </c>
       <c r="U68" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="V68" s="50" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="W68" s="81" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="X68" s="52"/>
       <c r="Y68" s="52"/>
@@ -4604,19 +4686,19 @@
       </c>
       <c r="T71" s="15"/>
       <c r="U71" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="V71" s="50" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="W71" s="81" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="X71" s="15"/>
       <c r="Y71" s="15"/>
       <c r="Z71" s="3"/>
       <c r="AA71" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AB71" s="3"/>
       <c r="AC71" s="3"/>
@@ -4628,7 +4710,7 @@
         <v>2</v>
       </c>
       <c r="AG71" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4798,7 +4880,7 @@
       <c r="AF75" s="3"/>
       <c r="AG75" s="46"/>
     </row>
-    <row r="76" spans="1:33" s="2" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
@@ -4827,9 +4909,7 @@
         <v>84</v>
       </c>
       <c r="V76" s="50"/>
-      <c r="W76" s="81" t="s">
-        <v>238</v>
-      </c>
+      <c r="W76" s="81"/>
       <c r="X76" s="56"/>
       <c r="Y76" s="56"/>
       <c r="Z76" s="3"/>
@@ -4955,9 +5035,11 @@
       <c r="U79" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="V79" s="50"/>
+      <c r="V79" s="50" t="s">
+        <v>268</v>
+      </c>
       <c r="W79" s="81" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="X79" s="53"/>
       <c r="Y79" s="53"/>
@@ -4975,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="AG79" s="46" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5265,7 +5347,7 @@
       <c r="AF86" s="3"/>
       <c r="AG86" s="46"/>
     </row>
-    <row r="87" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A87" s="15"/>
       <c r="B87" s="35"/>
       <c r="C87" s="54" t="s">
@@ -5291,12 +5373,16 @@
       </c>
       <c r="T87" s="35"/>
       <c r="U87" s="9"/>
-      <c r="V87" s="50"/>
-      <c r="W87" s="82"/>
+      <c r="V87" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="W87" s="81" t="s">
+        <v>236</v>
+      </c>
       <c r="X87" s="54"/>
       <c r="Y87" s="54"/>
       <c r="Z87" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AA87" s="3"/>
       <c r="AB87" s="3"/>
@@ -5309,7 +5395,7 @@
         <v>2</v>
       </c>
       <c r="AG87" s="53" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5353,7 +5439,7 @@
       <c r="AF88" s="3"/>
       <c r="AG88" s="3"/>
     </row>
-    <row r="89" spans="1:33" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15"/>
       <c r="B89" s="35"/>
       <c r="C89" s="15"/>
@@ -5381,14 +5467,10 @@
         <v>108</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="V89" s="50" t="s">
-        <v>230</v>
-      </c>
-      <c r="W89" s="81" t="s">
-        <v>242</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="V89" s="50"/>
+      <c r="W89" s="81"/>
       <c r="X89" s="53"/>
       <c r="Y89" s="53"/>
       <c r="Z89" s="3"/>
@@ -5505,10 +5587,10 @@
         <v>1</v>
       </c>
       <c r="T92" s="55" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="U92" s="9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="V92" s="50"/>
       <c r="W92" s="82"/>
@@ -6013,9 +6095,11 @@
       <c r="U105" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="V105" s="50"/>
+      <c r="V105" s="50" t="s">
+        <v>227</v>
+      </c>
       <c r="W105" s="81" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="X105" s="15"/>
       <c r="Y105" s="15"/>
@@ -6026,7 +6110,7 @@
       <c r="AB105" s="3"/>
       <c r="AC105" s="3"/>
       <c r="AD105" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AE105" s="46" t="s">
         <v>151</v>
@@ -6066,10 +6150,7 @@
         <v>108</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="V106" s="50" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="W106" s="82"/>
       <c r="X106" s="53"/>
@@ -6154,13 +6235,13 @@
         <v>108</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="V108" s="50" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="W108" s="81" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="X108" s="53"/>
       <c r="Y108" s="53"/>
@@ -6181,7 +6262,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="109" spans="1:34" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:34" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
@@ -6211,9 +6292,11 @@
       <c r="U109" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="V109" s="50"/>
+      <c r="V109" s="50" t="s">
+        <v>269</v>
+      </c>
       <c r="W109" s="81" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="X109" s="52"/>
       <c r="Y109" s="52"/>
@@ -6228,10 +6311,10 @@
         <v>151</v>
       </c>
       <c r="AF109" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG109" s="46" t="s">
-        <v>177</v>
+        <v>271</v>
       </c>
       <c r="AH109" s="12"/>
     </row>
@@ -6348,9 +6431,11 @@
       <c r="U112" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="V112" s="50"/>
+      <c r="V112" s="50" t="s">
+        <v>270</v>
+      </c>
       <c r="W112" s="81" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="X112" s="52"/>
       <c r="Y112" s="52"/>
@@ -6365,10 +6450,10 @@
       </c>
       <c r="AE112" s="3"/>
       <c r="AF112" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AG112" s="46" t="s">
-        <v>178</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6524,7 +6609,7 @@
       </c>
       <c r="V116" s="50"/>
       <c r="W116" s="81" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="X116" s="52"/>
       <c r="Y116" s="52"/>
@@ -6576,7 +6661,7 @@
       </c>
       <c r="V117" s="50"/>
       <c r="W117" s="81" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="X117" s="52"/>
       <c r="Y117" s="52"/>
@@ -6587,7 +6672,7 @@
       <c r="AB117" s="3"/>
       <c r="AC117" s="3"/>
       <c r="AD117" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AE117" s="3" t="s">
         <v>151</v>
@@ -6628,7 +6713,7 @@
       <c r="U118" s="12"/>
       <c r="V118" s="50"/>
       <c r="W118" s="81" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="X118" s="52"/>
       <c r="Y118" s="52"/>
@@ -6638,8 +6723,8 @@
       </c>
       <c r="AB118" s="3"/>
       <c r="AC118" s="3"/>
-      <c r="AD118" s="70" t="s">
-        <v>253</v>
+      <c r="AD118" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="AE118" s="3" t="s">
         <v>151</v>
@@ -6648,7 +6733,7 @@
         <v>2</v>
       </c>
       <c r="AG118" s="46" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -6682,13 +6767,13 @@
       </c>
       <c r="V119" s="50"/>
       <c r="W119" s="81" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="X119" s="52"/>
       <c r="Y119" s="52"/>
       <c r="Z119" s="3"/>
       <c r="AA119" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="AB119" s="3"/>
       <c r="AC119" s="3"/>
@@ -6700,7 +6785,7 @@
         <v>2</v>
       </c>
       <c r="AG119" s="46" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6713,7 +6798,7 @@
       <c r="G120" s="15"/>
       <c r="H120" s="15"/>
       <c r="I120" s="68" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J120" s="15"/>
       <c r="K120" s="15"/>
@@ -6731,7 +6816,7 @@
         <v>108</v>
       </c>
       <c r="U120" s="30" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="V120" s="50"/>
       <c r="W120" s="82"/>

</xml_diff>

<commit_message>
Korrigerat fel i nivån för multimediaentry.
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vårddokument.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vårddokument.xlsx
@@ -855,12 +855,6 @@
     <t>Vård- och omsorgsdokument.innehåll multimedia</t>
   </si>
   <si>
-    <t>Dokumentets innehåll i text</t>
-  </si>
-  <si>
-    <t>Länk till dokumentets innehåll i form av en multimediafil</t>
-  </si>
-  <si>
     <t>Händelsetidpunkt. Tidsangivelse för den händelse dokumentet gäller.</t>
   </si>
   <si>
@@ -887,6 +881,12 @@
   <si>
     <t>Kod för författarens befattning. Tillåtna värden från kodverk Befattning (OID 1.2.752.129.2.2.1.4) , se http://www.inera.se/Documents/Infrastrukturtjanster/Katalogtjanst_HSA/Innehll/hsa_innehall_befattning.pdf
 I de fall inte KV Befattning kan användas kan authorOtherRole användas för att ange befattning enligt annat kodverk</t>
+  </si>
+  <si>
+    <t>Dokumentets innehåll i text. . Något av clinicalDocumentNoteText eller multimediaEntry ska vara ifyllt.</t>
+  </si>
+  <si>
+    <t>Dokumentets innehåll i form av en multimediaobjekt, i form av antingen ett inbäddat objekt eller en länk till objektet. Något av clinicalDocumentNoteText eller multimediaEntry ska vara ifyllt.</t>
   </si>
 </sst>
 </file>
@@ -1559,9 +1559,9 @@
   </sheetPr>
   <dimension ref="A1:AT170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB127" sqref="AB127"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG114" sqref="AG114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2561,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="AG23" s="46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3053,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="AG34" s="53" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3288,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="AG39" s="46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3327,7 +3327,7 @@
       <c r="Y40" s="54"/>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
@@ -3337,7 +3337,7 @@
         <v>2</v>
       </c>
       <c r="AG40" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AH40" s="3"/>
     </row>
@@ -3378,7 +3378,7 @@
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
       <c r="AB41" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="AG41" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AH41" s="3"/>
     </row>
@@ -3430,7 +3430,7 @@
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
       <c r="AB42" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
@@ -3441,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="AG42" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AH42" s="3"/>
     </row>
@@ -6314,7 +6314,7 @@
         <v>2</v>
       </c>
       <c r="AG109" s="46" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="AH109" s="12"/>
     </row>
@@ -6439,10 +6439,9 @@
       </c>
       <c r="X112" s="52"/>
       <c r="Y112" s="52"/>
-      <c r="Z112" s="3" t="s">
+      <c r="AA112" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="AA112" s="3"/>
       <c r="AB112" s="3"/>
       <c r="AC112" s="3"/>
       <c r="AD112" s="3" t="s">
@@ -6453,7 +6452,7 @@
         <v>2</v>
       </c>
       <c r="AG112" s="46" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6486,7 +6485,6 @@
       <c r="W113" s="82"/>
       <c r="X113" s="52"/>
       <c r="Y113" s="52"/>
-      <c r="Z113" s="3"/>
       <c r="AA113" s="3"/>
       <c r="AB113" s="3"/>
       <c r="AC113" s="3"/>
@@ -6527,7 +6525,6 @@
       <c r="W114" s="82"/>
       <c r="X114" s="52"/>
       <c r="Y114" s="52"/>
-      <c r="Z114" s="3"/>
       <c r="AA114" s="3"/>
       <c r="AB114" s="3"/>
       <c r="AC114" s="3"/>
@@ -6568,7 +6565,6 @@
       <c r="W115" s="82"/>
       <c r="X115" s="52"/>
       <c r="Y115" s="52"/>
-      <c r="Z115" s="3"/>
       <c r="AA115" s="3"/>
       <c r="AB115" s="3"/>
       <c r="AC115" s="3"/>
@@ -6613,11 +6609,10 @@
       </c>
       <c r="X116" s="52"/>
       <c r="Y116" s="52"/>
-      <c r="Z116" s="3"/>
-      <c r="AA116" s="3" t="s">
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AB116" s="3"/>
       <c r="AC116" s="3"/>
       <c r="AD116" s="3"/>
       <c r="AE116" s="3" t="s">
@@ -6665,11 +6660,10 @@
       </c>
       <c r="X117" s="52"/>
       <c r="Y117" s="52"/>
-      <c r="Z117" s="3"/>
-      <c r="AA117" s="3" t="s">
+      <c r="AA117" s="3"/>
+      <c r="AB117" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AB117" s="3"/>
       <c r="AC117" s="3"/>
       <c r="AD117" s="3" t="s">
         <v>246</v>
@@ -6717,11 +6711,10 @@
       </c>
       <c r="X118" s="52"/>
       <c r="Y118" s="52"/>
-      <c r="Z118" s="3"/>
-      <c r="AA118" s="3" t="s">
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AB118" s="3"/>
       <c r="AC118" s="3"/>
       <c r="AD118" s="5" t="s">
         <v>247</v>
@@ -6771,11 +6764,10 @@
       </c>
       <c r="X119" s="52"/>
       <c r="Y119" s="52"/>
-      <c r="Z119" s="3"/>
-      <c r="AA119" s="3" t="s">
+      <c r="AA119" s="3"/>
+      <c r="AB119" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="AB119" s="3"/>
       <c r="AC119" s="3"/>
       <c r="AD119" s="3"/>
       <c r="AE119" s="3" t="s">
@@ -6822,7 +6814,6 @@
       <c r="W120" s="82"/>
       <c r="X120" s="55"/>
       <c r="Y120" s="55"/>
-      <c r="Z120" s="3"/>
       <c r="AA120" s="3"/>
       <c r="AB120" s="3"/>
       <c r="AC120" s="3"/>

</xml_diff>